<commit_message>
finalizaçao do 2º teste e atualizaçao dos documentos
</commit_message>
<xml_diff>
--- a/test/brew-day-tst.xlsx
+++ b/test/brew-day-tst.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -117,8 +117,8 @@
   <si>
     <t xml:space="preserve">Name: William ; 
 Last Name: Fabian ; 
-Email address: williamfabianmv@gmail.com _x005F_x0001_; 
-Confirm Email address: williamfabianmv@gmail.com _x005F_x0001_;
+Email address: williamfabianmv@gmail.com; 
+Confirm Email address: williamfabianmv@gmail.com;
 Password: (EM BRANCO); 
 Confirm Password: (EM BRANCO)</t>
   </si>
@@ -135,7 +135,7 @@
     <t xml:space="preserve">CT4</t>
   </si>
   <si>
-    <t xml:space="preserve">Email address: _x005F_x0001_williamfabianmv@gmail.com ; 
+    <t xml:space="preserve">Email address: williamfabianmv@gmail.com ; 
 Password: 1234; </t>
   </si>
   <si>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">CT5</t>
   </si>
   <si>
-    <t xml:space="preserve">Email address: _x005F_x0001_will@gmail.com ; 
+    <t xml:space="preserve">Email address: will@gmail.com ; 
 Password: 1234; </t>
   </si>
   <si>
@@ -173,45 +173,12 @@
     <t xml:space="preserve">CT7</t>
   </si>
   <si>
-    <t xml:space="preserve">CT8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT9</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Name: will ; 
+    <t xml:space="preserve">Name: will ; 
 Last Name: will ; 
 Email address: will@gmail.com; 
-Confirm Email address: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">will@gmail.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">; 
+Confirm Email address: will@gmail.com; 
 Password: 000; 
 Confirm Password: 000</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Retorno á tela inicial</t>
@@ -242,6 +209,9 @@
 Password: 000; </t>
   </si>
   <si>
+    <t xml:space="preserve">CT8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Additives Name: corante
 Quantity: 1
 GRAMS</t>
@@ -253,6 +223,9 @@
     <t xml:space="preserve">Registro adicionado com sucesso mas sem confirmação</t>
   </si>
   <si>
+    <t xml:space="preserve">CT9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sistema informar ocorrência de Ingrediente repetido</t>
   </si>
   <si>
@@ -287,6 +260,11 @@
     <t xml:space="preserve">C14</t>
   </si>
   <si>
+    <t xml:space="preserve">Filter Name: Barril
+Quantity: 2
+Litle(l)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Confirmação de adição e Equipamento adicionado no banco de dados</t>
   </si>
   <si>
@@ -296,6 +274,11 @@
     <t xml:space="preserve">C16</t>
   </si>
   <si>
+    <t xml:space="preserve">Filter Name: (EM BRANCO)
+Quantity: 2
+Litle(l)</t>
+  </si>
+  <si>
     <t xml:space="preserve">C17</t>
   </si>
   <si>
@@ -314,27 +297,11 @@
     <t xml:space="preserve">C20</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Recipes Name: Receita teste
+    <t xml:space="preserve">Recipes Name: Receita teste
 Type Brew: USER
 Malt: Malte Grao (kg)    Quantity: 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Hop: Lupulo Persa (gr)    Quantity: 1
+Hop: Lupulo Persa (gr)    Quantity: 1
 Additive:  corante (gr)    Quantity: 1</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Confirmação de adição e Receita adicionado no banco de dados</t>
@@ -346,27 +313,11 @@
     <t xml:space="preserve">C22</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Recipes Name: (EM BRANCO)
+    <t xml:space="preserve">Recipes Name: (EM BRANCO)
 Type Brew: USER
 Malt: Malte Grao (kg)    Quantity: 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Hop: Lupulo Persa (gr)    Quantity: 1
+Hop: Lupulo Persa (gr)    Quantity: 1
 Additive:  corante (gr)    Quantity: 1</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">invalid literal for int() with base 10: '' </t>
@@ -385,6 +336,18 @@
   </si>
   <si>
     <t xml:space="preserve">Receita Deletada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmação de produção e Ingrediente subtraídos no banco de dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aviso de falta de um ou mais ingredientes</t>
   </si>
 </sst>
 </file>
@@ -437,7 +400,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,7 +410,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF37B70"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FFF68E76"/>
       </patternFill>
     </fill>
     <fill>
@@ -466,6 +429,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7DA7D8"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF68E76"/>
+        <bgColor rgb="FFF37B70"/>
       </patternFill>
     </fill>
   </fills>
@@ -510,7 +479,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -591,14 +560,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -619,20 +580,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -691,7 +652,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFF9AE"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFF68E76"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -720,10 +681,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -898,22 +859,6 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -930,10 +875,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -975,38 +920,38 @@
       <c r="A2" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>34</v>
+      <c r="E2" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>36</v>
+      <c r="E3" s="21" t="s">
+        <v>34</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="11" t="s">
@@ -1021,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>15</v>
@@ -1042,13 +987,13 @@
         <v>18</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="18" t="s">
@@ -1063,7 +1008,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>25</v>
@@ -1112,17 +1057,17 @@
       <c r="A9" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="E9" s="24" t="s">
         <v>42</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,16 +1075,16 @@
         <v>43110</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,7 +1131,7 @@
       <c r="C13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="19" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="19" t="s">
@@ -1203,62 +1148,62 @@
       <c r="C14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="25" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="29" t="s">
+      <c r="C15" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="30" t="s">
+      <c r="B16" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>29</v>
+      <c r="E16" s="27" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="29" t="s">
+      <c r="B17" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>29</v>
+      <c r="E17" s="28" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,13 +1211,13 @@
         <v>43110</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>59</v>
+      <c r="D18" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>29</v>
@@ -1283,12 +1228,12 @@
         <v>43110</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="25" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="19" t="s">
@@ -1300,13 +1245,13 @@
         <v>43110</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>62</v>
+      <c r="D20" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>29</v>
@@ -1316,17 +1261,17 @@
       <c r="A21" s="5" t="n">
         <v>43110</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="26" t="s">
+      <c r="B21" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>43</v>
+      <c r="C21" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,16 +1279,16 @@
         <v>43110</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,68 +1296,107 @@
         <v>43110</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="31" t="s">
-        <v>69</v>
+      <c r="E23" s="29" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="32" t="s">
-        <v>70</v>
+      <c r="A24" s="5" t="n">
+        <v>43110</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="32" t="s">
-        <v>72</v>
+      <c r="A25" s="5" t="n">
+        <v>43110</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>59</v>
+      <c r="D25" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="32" t="s">
-        <v>73</v>
+      <c r="A26" s="5" t="n">
+        <v>43110</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>75</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>43110</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>43110</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="will@gmail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="will@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>